<commit_message>
Multiple session error - handle. Bug fixes!!
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790D7B51-20C5-4A0B-AE02-59E934DB6D5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76FADF8-960A-49E5-BAEF-39D13A22A483}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="6" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -1568,40 +1568,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1661,15 +1631,6 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1683,6 +1644,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2001,7 +2001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DA82F7-BAEB-47DA-A709-D2C1E8B67183}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
@@ -2263,7 +2263,7 @@
   <dimension ref="A1:XFD23"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E6" sqref="A1:XFD1048576"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2275,18 +2275,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
     </row>
     <row r="2" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
@@ -2301,28 +2301,28 @@
       <c r="J2" s="24"/>
     </row>
     <row r="3" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="59"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="57"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="47"/>
     </row>
     <row r="4" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
@@ -2337,23 +2337,23 @@
       <c r="J4" s="24"/>
     </row>
     <row r="5" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="60" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="60"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="57"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+      <c r="H5" s="50"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="47"/>
     </row>
     <row r="6" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
+      <c r="A6" s="61"/>
       <c r="B6" s="19"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -2365,129 +2365,129 @@
       <c r="J6" s="24"/>
     </row>
     <row r="7" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="61"/>
+      <c r="B7" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="57"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="I7" s="50"/>
+      <c r="J7" s="47"/>
     </row>
     <row r="8" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="A8" s="61"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="57"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="47"/>
     </row>
     <row r="9" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
+      <c r="A9" s="61"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="52"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="67"/>
-      <c r="J9" s="68"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="55"/>
     </row>
     <row r="10" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="61"/>
+      <c r="B10" s="59" t="s">
         <v>185</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="31" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="31" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="57"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="47"/>
     </row>
     <row r="11" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="31" t="s">
         <v>189</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="I11" s="59"/>
-      <c r="J11" s="57"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="47"/>
     </row>
     <row r="12" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="35" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="57"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="47"/>
     </row>
     <row r="13" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="35" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="51" t="s">
         <v>205</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="57"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="47"/>
     </row>
     <row r="14" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
+      <c r="A14" s="61"/>
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
@@ -2495,80 +2495,80 @@
       <c r="F14" s="20"/>
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="42"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
     </row>
     <row r="16" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="35" t="s">
+      <c r="A16" s="61"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
     </row>
     <row r="17" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="62"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="35" t="s">
+      <c r="A17" s="61"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="31" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="62"/>
-      <c r="B18" s="40"/>
-      <c r="C18" s="34" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="31" t="s">
         <v>221</v>
       </c>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="I18" s="35" t="s">
+      <c r="I18" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="J18" s="35" t="s">
+      <c r="J18" s="31" t="s">
         <v>226</v>
       </c>
       <c r="K18" s="21"/>
@@ -18947,22 +18947,22 @@
       <c r="XFD18" s="21"/>
     </row>
     <row r="19" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="62"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="34" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="31" t="s">
         <v>227</v>
       </c>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
       <c r="K19" s="21"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
@@ -35339,64 +35339,64 @@
       <c r="XFD19" s="21"/>
     </row>
     <row r="20" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="62"/>
+      <c r="A20" s="61"/>
       <c r="B20" s="19"/>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="66"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="62"/>
-      <c r="B21" s="39" t="s">
+      <c r="A21" s="61"/>
+      <c r="B21" s="63" t="s">
         <v>207</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="31" t="s">
         <v>228</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="59"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="60"/>
-      <c r="H21" s="60"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="57"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
+      <c r="I21" s="50"/>
+      <c r="J21" s="47"/>
     </row>
     <row r="22" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="62"/>
-      <c r="B22" s="40"/>
-      <c r="C22" s="35" t="s">
+      <c r="A22" s="61"/>
+      <c r="B22" s="64"/>
+      <c r="C22" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="60"/>
-      <c r="H22" s="60"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="57"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="50"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="50"/>
+      <c r="J22" s="47"/>
     </row>
     <row r="23" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="63"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="35" t="s">
+      <c r="A23" s="62"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="31" t="s">
         <v>229</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="E23" s="53"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="54"/>
-      <c r="I23" s="54"/>
-      <c r="J23" s="55"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -35428,13 +35428,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
@@ -35444,19 +35444,19 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>240</v>
       </c>
     </row>
@@ -35468,122 +35468,122 @@
       <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="66" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="C5" s="59"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="57"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="47"/>
     </row>
     <row r="6" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="19"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="59" t="s">
         <v>243</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="31" t="s">
         <v>244</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="56"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="46"/>
     </row>
     <row r="8" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="E8" s="56"/>
+      <c r="E8" s="46"/>
     </row>
     <row r="9" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="57"/>
+      <c r="E9" s="47"/>
     </row>
     <row r="10" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="33" t="s">
+      <c r="A10" s="67"/>
+      <c r="B10" s="59" t="s">
         <v>248</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="56"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="46"/>
     </row>
     <row r="11" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="33"/>
-      <c r="C11" s="34" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="31" t="s">
         <v>251</v>
       </c>
-      <c r="E11" s="56"/>
+      <c r="E11" s="46"/>
     </row>
     <row r="12" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
+      <c r="A12" s="67"/>
       <c r="B12" s="19"/>
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
-      <c r="E12" s="57"/>
+      <c r="E12" s="47"/>
     </row>
     <row r="13" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="39" t="s">
+      <c r="A13" s="67"/>
+      <c r="B13" s="63" t="s">
         <v>247</v>
       </c>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="31" t="s">
         <v>253</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="31" t="s">
         <v>252</v>
       </c>
-      <c r="E13" s="56"/>
+      <c r="E13" s="46"/>
     </row>
     <row r="14" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="35" t="s">
+      <c r="A14" s="67"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="31" t="s">
         <v>254</v>
       </c>
-      <c r="D14" s="35"/>
-      <c r="E14" s="56"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="46"/>
     </row>
     <row r="15" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="35" t="s">
+      <c r="A15" s="67"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="E15" s="56"/>
+      <c r="E15" s="46"/>
     </row>
     <row r="16" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="35" t="s">
+      <c r="A16" s="67"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="56"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="46"/>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
       <c r="H16" s="21"/>
@@ -51960,15 +51960,15 @@
       <c r="XEY16" s="21"/>
     </row>
     <row r="17" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="34" t="s">
+      <c r="A17" s="68"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="30" t="s">
         <v>259</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="31" t="s">
         <v>258</v>
       </c>
-      <c r="E17" s="58"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
       <c r="H17" s="21"/>
@@ -68362,7 +68362,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -68373,20 +68373,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="59" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
@@ -68403,26 +68403,26 @@
       <c r="L2" s="24"/>
     </row>
     <row r="3" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>265</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="31" t="s">
         <v>266</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="45"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
@@ -68439,25 +68439,25 @@
       <c r="L4" s="24"/>
     </row>
     <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="66" t="s">
         <v>268</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="45"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="19"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -68471,160 +68471,160 @@
       <c r="L6" s="24"/>
     </row>
     <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="59" t="s">
         <v>261</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="31" t="s">
         <v>269</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="35"/>
     </row>
     <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="30" t="s">
         <v>270</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="31" t="s">
         <v>271</v>
       </c>
-      <c r="E8" s="43"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="45"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="34"/>
+      <c r="G8" s="34"/>
+      <c r="H8" s="34"/>
+      <c r="I8" s="34"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="52"/>
-      <c r="L9" s="42"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="32"/>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="67"/>
+      <c r="B10" s="63" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="35" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="31" t="s">
         <v>274</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="35" t="s">
+      <c r="A12" s="67"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="31" t="s">
         <v>276</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="34" t="s">
+      <c r="A13" s="67"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="30" t="s">
         <v>277</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="31" t="s">
         <v>279</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="31" t="s">
         <v>280</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="31" t="s">
         <v>281</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="31" t="s">
         <v>282</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="31" t="s">
         <v>283</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="I13" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="J13" s="35" t="s">
+      <c r="J13" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="K13" s="31" t="s">
         <v>286</v>
       </c>
-      <c r="L13" s="35" t="s">
+      <c r="L13" s="31" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="34" t="s">
+      <c r="A14" s="68"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="30" t="s">
         <v>278</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="31" t="s">
         <v>288</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -68654,13 +68654,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="59" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
@@ -68670,19 +68670,19 @@
       <c r="E2" s="24"/>
     </row>
     <row r="3" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>291</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>292</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="31" t="s">
         <v>293</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="31" t="s">
         <v>294</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="31" t="s">
         <v>295</v>
       </c>
     </row>
@@ -68694,142 +68694,142 @@
       <c r="E4" s="24"/>
     </row>
     <row r="5" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="66" t="s">
         <v>296</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>297</v>
       </c>
-      <c r="C5" s="43"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="45"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="19"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
       <c r="E6" s="24"/>
     </row>
     <row r="7" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="59" t="s">
         <v>298</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="31" t="s">
         <v>299</v>
       </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="47"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="37"/>
     </row>
     <row r="8" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="37"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="A8" s="67"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="30" t="s">
         <v>300</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="31" t="s">
         <v>301</v>
       </c>
-      <c r="E8" s="47"/>
+      <c r="E8" s="37"/>
     </row>
     <row r="9" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37"/>
+      <c r="A9" s="67"/>
       <c r="B9" s="19"/>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="45"/>
+      <c r="E9" s="35"/>
     </row>
     <row r="10" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
-      <c r="B10" s="39" t="s">
+      <c r="A10" s="67"/>
+      <c r="B10" s="63" t="s">
         <v>302</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="31" t="s">
         <v>304</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="31" t="s">
         <v>305</v>
       </c>
-      <c r="E10" s="47"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="35" t="s">
+      <c r="A11" s="67"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="31" t="s">
         <v>306</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="31" t="s">
         <v>307</v>
       </c>
-      <c r="E11" s="47"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="35" t="s">
+      <c r="A12" s="67"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="31" t="s">
         <v>308</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="47"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="37"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="35" t="s">
+      <c r="A13" s="67"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="31" t="s">
         <v>309</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="47"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="37"/>
     </row>
     <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37"/>
+      <c r="A14" s="67"/>
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
-      <c r="E14" s="45"/>
+      <c r="E14" s="35"/>
     </row>
     <row r="15" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="67"/>
+      <c r="B15" s="63" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="31" t="s">
         <v>310</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="31" t="s">
         <v>311</v>
       </c>
-      <c r="E15" s="47"/>
+      <c r="E15" s="37"/>
     </row>
     <row r="16" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="35" t="s">
+      <c r="A16" s="67"/>
+      <c r="B16" s="64"/>
+      <c r="C16" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="31" t="s">
         <v>313</v>
       </c>
-      <c r="E16" s="47"/>
+      <c r="E16" s="37"/>
     </row>
     <row r="17" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="37"/>
-      <c r="B17" s="40"/>
-      <c r="C17" s="35" t="s">
+      <c r="A17" s="67"/>
+      <c r="B17" s="64"/>
+      <c r="C17" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="47"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="35" t="s">
+      <c r="A18" s="68"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="31" t="s">
         <v>315</v>
       </c>
-      <c r="D18" s="35"/>
-      <c r="E18" s="46"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -68860,12 +68860,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="59" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
@@ -68874,16 +68874,16 @@
       <c r="D2" s="24"/>
     </row>
     <row r="3" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="31" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="D3" s="48"/>
+      <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21"/>
@@ -68892,38 +68892,38 @@
       <c r="D4" s="24"/>
     </row>
     <row r="5" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="66" t="s">
         <v>320</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
+      <c r="A6" s="67"/>
       <c r="B6" s="19"/>
       <c r="C6" s="21"/>
       <c r="D6" s="24"/>
     </row>
     <row r="7" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="33" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="59" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="31" t="s">
         <v>323</v>
       </c>
-      <c r="D7" s="35"/>
+      <c r="D7" s="31"/>
     </row>
     <row r="8" spans="1:4" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="34" t="s">
+      <c r="A8" s="68"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="31" t="s">
         <v>325</v>
       </c>
     </row>
@@ -70092,9 +70092,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718F9279-C340-4770-88F1-01842C5185FC}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -70401,7 +70401,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="56" t="s">
         <v>157</v>
       </c>
       <c r="B1" s="25" t="s">
@@ -70436,8 +70436,8 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30" t="s">
+      <c r="A2" s="56"/>
+      <c r="B2" s="56" t="s">
         <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -70465,8 +70465,8 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="25" t="s">
         <v>178</v>
       </c>
@@ -70482,8 +70482,8 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30" t="s">
+      <c r="A4" s="56"/>
+      <c r="B4" s="56" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -70501,8 +70501,8 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="56"/>
+      <c r="B5" s="56"/>
       <c r="C5" s="25" t="s">
         <v>178</v>
       </c>
@@ -70532,8 +70532,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30" t="s">
+      <c r="A6" s="56"/>
+      <c r="B6" s="56" t="s">
         <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -70551,8 +70551,8 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="56"/>
       <c r="C7" s="25" t="s">
         <v>178</v>
       </c>
@@ -70570,7 +70570,7 @@
       <c r="M7" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="56" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="25" t="s">
@@ -70591,7 +70591,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30"/>
+      <c r="A10" s="56"/>
       <c r="B10" s="25" t="s">
         <v>160</v>
       </c>
@@ -70612,8 +70612,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="22" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30" t="s">
+      <c r="A11" s="56"/>
+      <c r="B11" s="56" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -70629,8 +70629,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="56"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="25" t="s">
         <v>178</v>
       </c>
@@ -70648,7 +70648,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="56" t="s">
         <v>164</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -70683,8 +70683,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30" t="s">
+      <c r="A15" s="56"/>
+      <c r="B15" s="56" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -70702,8 +70702,8 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="56"/>
       <c r="C16" s="25" t="s">
         <v>178</v>
       </c>
@@ -70729,7 +70729,7 @@
       <c r="K16" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="56" t="s">
         <v>168</v>
       </c>
       <c r="B18" s="25" t="s">
@@ -70749,8 +70749,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30" t="s">
+      <c r="A19" s="56"/>
+      <c r="B19" s="56" t="s">
         <v>169</v>
       </c>
       <c r="C19" s="29" t="s">
@@ -70765,8 +70765,8 @@
       <c r="F19" s="29"/>
     </row>
     <row r="20" spans="1:6" s="28" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="25" t="s">
         <v>178</v>
       </c>
@@ -70777,8 +70777,8 @@
       <c r="F20" s="29"/>
     </row>
     <row r="21" spans="1:6" s="28" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31" t="s">
+      <c r="A21" s="56"/>
+      <c r="B21" s="57" t="s">
         <v>170</v>
       </c>
       <c r="C21" s="29" t="s">
@@ -70793,8 +70793,8 @@
       <c r="F21" s="29"/>
     </row>
     <row r="22" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="56"/>
+      <c r="B22" s="58"/>
       <c r="C22" s="25" t="s">
         <v>178</v>
       </c>

</xml_diff>